<commit_message>
Mise à jour générale
Mise à jour du 8 août 2020.
</commit_message>
<xml_diff>
--- a/Coronavirus (v2.4.2).xlsx
+++ b/Coronavirus (v2.4.2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\druon\Desktop\LOL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA37DE-B481-42F9-9E70-DDA4C580B440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1213DB6-1991-4831-BAAA-26D0416CF019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C74FB7AA-F2FE-4EBA-A853-66368F783162}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="295">
   <si>
     <t>www.worldometers.info/coronavirus</t>
   </si>
@@ -740,9 +740,6 @@
     <t>5,07 M</t>
   </si>
   <si>
-    <t>12,6 M</t>
-  </si>
-  <si>
     <t>2,60 M</t>
   </si>
   <si>
@@ -1049,66 +1046,73 @@
     <t>3 mois et 29 jours</t>
   </si>
   <si>
-    <t>[2]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="5"/>
-        <rFont val="Century Schoolbook"/>
-        <family val="1"/>
-      </rPr>
-      <t>[2]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Century Schoolbook"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Les données de l'Italie, étant toutes augmentées de 21, j'ai préféré faire une formule qui calcule automatiquement le résultat en fonction des anciennes données. Ce sont donc ces anciennes données.</t>
-    </r>
-  </si>
-  <si>
-    <t>TOP 10 des pays les plus touchés (au 31 juillet) :</t>
-  </si>
-  <si>
-    <t>333 ms</t>
-  </si>
-  <si>
-    <t>15,3 s</t>
-  </si>
-  <si>
-    <t>58,5 M</t>
-  </si>
-  <si>
-    <t>18,8 M</t>
-  </si>
-  <si>
-    <t>28,1 M</t>
-  </si>
-  <si>
-    <t>6,67 M</t>
-  </si>
-  <si>
-    <t>Iran</t>
-  </si>
-  <si>
-    <t>1 m 22</t>
-  </si>
-  <si>
-    <t>2 h 24 m</t>
-  </si>
-  <si>
-    <t>2,95 M</t>
-  </si>
-  <si>
-    <t>968 K</t>
-  </si>
-  <si>
-    <t>1,62 M</t>
+    <t>5,99 M</t>
+  </si>
+  <si>
+    <t>6,06 M</t>
+  </si>
+  <si>
+    <t>6,05 M</t>
+  </si>
+  <si>
+    <t>6,07 M</t>
+  </si>
+  <si>
+    <t>6,09 M</t>
+  </si>
+  <si>
+    <t>6,18 M</t>
+  </si>
+  <si>
+    <t>6,27 M</t>
+  </si>
+  <si>
+    <t>TOP 10 des pays les plus touchés (au 7 août) :</t>
+  </si>
+  <si>
+    <t>63,8 M</t>
+  </si>
+  <si>
+    <t>13,2 M</t>
+  </si>
+  <si>
+    <t>22,7 M</t>
+  </si>
+  <si>
+    <t>30,0 M</t>
+  </si>
+  <si>
+    <t>3,18 M</t>
+  </si>
+  <si>
+    <t>2,52 M</t>
+  </si>
+  <si>
+    <t>1,05 M</t>
+  </si>
+  <si>
+    <t>1,78 M</t>
+  </si>
+  <si>
+    <t>Colombie</t>
+  </si>
+  <si>
+    <t>7,06 M</t>
+  </si>
+  <si>
+    <t>4,08 M</t>
+  </si>
+  <si>
+    <t>341 ms</t>
+  </si>
+  <si>
+    <t>15,0 s</t>
+  </si>
+  <si>
+    <t>1 m 01 s</t>
+  </si>
+  <si>
+    <t>2 h 40 m</t>
   </si>
 </sst>
 </file>
@@ -1683,10 +1687,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'(DB) Données Complètes'!$A$2:$A$183</c:f>
+              <c:f>'(DB) Données Complètes'!$A$2:$A$190</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>43862</c:v>
                 </c:pt>
@@ -2232,16 +2236,37 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'(DB) Données Complètes'!$C$2:$C$183</c:f>
+              <c:f>'(DB) Données Complètes'!$C$2:$C$190</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:formatCode>_ * #.##0_ ;_ * \-#.##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>13000</c:v>
                 </c:pt>
@@ -2787,6 +2812,27 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>5915000</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>5997000</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>6067000</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>6057000</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>6074000</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>6098000</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>6182000</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>6271000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3138,10 +3184,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Données!$A$2:$A$183</c:f>
+              <c:f>Données!$A$2:$A$190</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>43862</c:v>
                 </c:pt>
@@ -3687,16 +3733,37 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Données!$F$2:$F$183</c:f>
+              <c:f>Données!$F$2:$F$190</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4242,6 +4309,27 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>110199</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>112704</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>115669</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>118704</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>124438</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>127390</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>131477</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>135981</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4281,10 +4369,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Données!$A$2:$A$183</c:f>
+              <c:f>Données!$A$2:$A$190</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>43862</c:v>
                 </c:pt>
@@ -4830,16 +4918,37 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Données!$E$2:$E$183</c:f>
+              <c:f>Données!$E$2:$E$190</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5385,6 +5494,27 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>12422</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>12457</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>12456</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>12474</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>12482</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>12646</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>12694</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>12924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5424,10 +5554,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Données!$A$2:$A$183</c:f>
+              <c:f>Données!$A$2:$A$190</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>43862</c:v>
                 </c:pt>
@@ -5973,16 +6103,37 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'(DB) Données Complètes'!$D$2:$D$183</c:f>
+              <c:f>'(DB) Données Complètes'!$D$2:$D$190</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:formatCode>_ * #.##0_ ;_ * \-#.##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6489,6 +6640,27 @@
                 </c:pt>
                 <c:pt idx="179">
                   <c:v>73458</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>74652</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>75773</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>78835</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>79720</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>81264</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>82651</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>84761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6840,10 +7012,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'(DB) Données Complètes'!$A$2:$A$183</c:f>
+              <c:f>'(DB) Données Complètes'!$A$2:$A$190</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>43862</c:v>
                 </c:pt>
@@ -7389,16 +7561,37 @@
                 </c:pt>
                 <c:pt idx="181">
                   <c:v>44043</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>44045</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>44046</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>44047</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>44048</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>44049</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>44050</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'(DB) Données Complètes'!$D$2:$D$183</c:f>
+              <c:f>'(DB) Données Complètes'!$D$2:$D$190</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="182"/>
+                <c:formatCode>_ * #.##0_ ;_ * \-#.##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
+                <c:ptCount val="189"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -7905,6 +8098,27 @@
                 </c:pt>
                 <c:pt idx="179">
                   <c:v>73458</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>74652</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>75773</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>78835</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>79720</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>81264</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>82651</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>84761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10247,7 +10461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2733ED11-6989-4273-BE69-0BA9E3873236}">
-  <dimension ref="A1:O183"/>
+  <dimension ref="A1:O190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -10469,7 +10683,7 @@
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -10539,13 +10753,13 @@
         <v>6</v>
       </c>
       <c r="I9" s="4">
-        <v>17752831</v>
+        <v>19532532</v>
       </c>
       <c r="J9" s="4">
-        <v>682392</v>
+        <v>723184</v>
       </c>
       <c r="K9" s="5">
-        <v>5915399</v>
+        <v>6271494</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>17</v>
@@ -10554,10 +10768,10 @@
         <v>17</v>
       </c>
       <c r="N9" s="15" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -10586,19 +10800,19 @@
         <v>11</v>
       </c>
       <c r="I10" s="27">
-        <v>4705889</v>
+        <v>5095524</v>
       </c>
       <c r="J10" s="27">
-        <v>156747</v>
+        <v>164094</v>
       </c>
       <c r="K10" s="21">
-        <v>2221570</v>
+        <v>2314463</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="M10" s="31">
-        <v>17.690000000000001</v>
+        <v>19.29</v>
       </c>
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
@@ -10629,19 +10843,19 @@
         <v>13</v>
       </c>
       <c r="I11" s="28">
-        <v>2666298</v>
+        <v>2967064</v>
       </c>
       <c r="J11" s="28">
-        <v>92568</v>
+        <v>99702</v>
       </c>
       <c r="K11" s="22">
-        <v>689679</v>
+        <v>798968</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>170</v>
+        <v>281</v>
       </c>
       <c r="M11" s="32">
-        <v>5.92</v>
+        <v>6.2</v>
       </c>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
@@ -10672,19 +10886,19 @@
         <v>18</v>
       </c>
       <c r="I12" s="71">
-        <v>1697054</v>
+        <v>2086864</v>
       </c>
       <c r="J12" s="71">
-        <v>36551</v>
+        <v>42578</v>
       </c>
       <c r="K12" s="23">
-        <v>564856</v>
+        <v>616617</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="M12" s="30">
-        <v>1.36</v>
+        <v>1.64</v>
       </c>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
@@ -10715,19 +10929,19 @@
         <v>12</v>
       </c>
       <c r="I13" s="26">
-        <v>839981</v>
+        <v>877135</v>
       </c>
       <c r="J13" s="26">
-        <v>13963</v>
+        <v>14725</v>
       </c>
       <c r="K13" s="25">
-        <v>187608</v>
+        <v>178818</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="M13" s="33">
-        <v>19.29</v>
+        <v>20.58</v>
       </c>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
@@ -10758,19 +10972,19 @@
         <v>165</v>
       </c>
       <c r="I14" s="4">
-        <v>493183</v>
+        <v>545476</v>
       </c>
       <c r="J14" s="4">
-        <v>8005</v>
+        <v>9909</v>
       </c>
       <c r="K14" s="5">
-        <v>159007</v>
+        <v>140808</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M14" s="29">
-        <v>4.9800000000000004</v>
+        <v>5.36</v>
       </c>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
@@ -10797,23 +11011,23 @@
       <c r="G15" s="5">
         <v>6</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="I15" s="26">
-        <v>416179</v>
-      </c>
-      <c r="J15" s="26">
-        <v>46000</v>
-      </c>
-      <c r="K15" s="25">
-        <v>97992</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>286</v>
-      </c>
-      <c r="M15" s="33">
-        <v>0.75</v>
+      <c r="H15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="4">
+        <v>463875</v>
+      </c>
+      <c r="J15" s="4">
+        <v>20649</v>
+      </c>
+      <c r="K15" s="5">
+        <v>128894</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="M15" s="29">
+        <v>7.64</v>
       </c>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
@@ -10841,23 +11055,23 @@
       <c r="G16" s="5">
         <v>7</v>
       </c>
-      <c r="H16" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="4">
-        <v>414735</v>
-      </c>
-      <c r="J16" s="4">
-        <v>19217</v>
-      </c>
-      <c r="K16" s="5">
-        <v>108391</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="M16" s="29">
-        <v>7.11</v>
+      <c r="H16" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" s="26">
+        <v>462690</v>
+      </c>
+      <c r="J16" s="26">
+        <v>50517</v>
+      </c>
+      <c r="K16" s="25">
+        <v>103325</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="M16" s="33">
+        <v>0.81</v>
       </c>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
@@ -10889,19 +11103,19 @@
         <v>49</v>
       </c>
       <c r="I17" s="4">
-        <v>355667</v>
+        <v>368825</v>
       </c>
       <c r="J17" s="4">
-        <v>9457</v>
+        <v>9958</v>
       </c>
       <c r="K17" s="5">
-        <v>17883</v>
+        <v>16699</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>287</v>
       </c>
       <c r="M17" s="29">
-        <v>8.48</v>
+        <v>9.33</v>
       </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
@@ -10930,22 +11144,22 @@
         <v>9</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>7</v>
+        <v>288</v>
       </c>
       <c r="I18" s="26">
-        <v>335602</v>
+        <v>367196</v>
       </c>
       <c r="J18" s="26">
-        <v>28445</v>
+        <v>12250</v>
       </c>
       <c r="K18" s="25">
-        <v>110199</v>
+        <v>156451</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>281</v>
+        <v>206</v>
       </c>
       <c r="M18" s="33">
-        <v>14.28</v>
+        <v>3.61</v>
       </c>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
@@ -10974,22 +11188,22 @@
         <v>10</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>282</v>
+        <v>7</v>
       </c>
       <c r="I19" s="26">
-        <v>304204</v>
+        <v>361442</v>
       </c>
       <c r="J19" s="26">
-        <v>16766</v>
+        <v>28503</v>
       </c>
       <c r="K19" s="25">
-        <v>23919</v>
+        <v>135981</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>220</v>
+        <v>289</v>
       </c>
       <c r="M19" s="33">
-        <v>2.92</v>
+        <v>15.1</v>
       </c>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
@@ -11053,25 +11267,25 @@
         <v>72</v>
       </c>
       <c r="I21" s="5">
-        <v>187919</v>
+        <v>197921</v>
       </c>
       <c r="J21" s="5">
-        <v>30265</v>
+        <v>30324</v>
       </c>
       <c r="K21" s="5">
-        <v>76154</v>
+        <v>84761</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>142</v>
+        <v>290</v>
       </c>
       <c r="M21" s="15">
-        <v>4.5599999999999996</v>
+        <v>6.26</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -11415,7 +11629,7 @@
         <v>43898</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C38" s="8">
         <v>1178</v>
@@ -11479,7 +11693,7 @@
         <v>43901</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="8">
         <v>2221</v>
@@ -11522,7 +11736,7 @@
         <v>43903</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C43" s="8">
         <v>3570</v>
@@ -11544,7 +11758,7 @@
         <v>43904</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C44" s="8">
         <v>4396</v>
@@ -11566,7 +11780,7 @@
         <v>43905</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="8">
         <v>5284</v>
@@ -11588,7 +11802,7 @@
         <v>43906</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C46" s="8">
         <v>6473</v>
@@ -11764,7 +11978,7 @@
         <v>43914</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C54" s="8">
         <v>17923</v>
@@ -11786,7 +12000,7 @@
         <v>43915</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C55" s="8">
         <v>20002</v>
@@ -11808,7 +12022,7 @@
         <v>43916</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C56" s="8">
         <v>22511</v>
@@ -11852,7 +12066,7 @@
         <v>43918</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" s="8">
         <v>29561</v>
@@ -11874,7 +12088,7 @@
         <v>43919</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C59" s="8">
         <v>30366</v>
@@ -11896,7 +12110,7 @@
         <v>43920</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C60" s="8">
         <v>33599</v>
@@ -11918,7 +12132,7 @@
         <v>43921</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C61" s="8">
         <v>39161</v>
@@ -11940,7 +12154,7 @@
         <v>43922</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" s="8">
         <v>42022</v>
@@ -11962,7 +12176,7 @@
         <v>43923</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C63" s="8">
         <v>41290</v>
@@ -11984,7 +12198,7 @@
         <v>43924</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C64" s="8">
         <v>43823</v>
@@ -12001,12 +12215,12 @@
       </c>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>43925</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" s="8">
         <v>45607</v>
@@ -12023,12 +12237,12 @@
       </c>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>43926</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="8">
         <v>46217</v>
@@ -12045,12 +12259,12 @@
       </c>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>43927</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C67" s="8">
         <v>48229</v>
@@ -12067,12 +12281,12 @@
       </c>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>43928</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C68" s="8">
         <v>48502</v>
@@ -12089,12 +12303,12 @@
       </c>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>43929</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69" s="8">
         <v>49925</v>
@@ -12111,7 +12325,7 @@
       </c>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>43930</v>
       </c>
@@ -12133,12 +12347,12 @@
       </c>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>43931</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C71" s="8">
         <v>52547</v>
@@ -12155,7 +12369,7 @@
       </c>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>43932</v>
       </c>
@@ -12176,16 +12390,14 @@
         <v>87312</v>
       </c>
       <c r="G72" s="8"/>
-      <c r="H72" s="73" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="73"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>43933</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C73" s="8">
         <v>53824</v>
@@ -12194,24 +12406,22 @@
         <f t="shared" si="0"/>
         <v>257</v>
       </c>
-      <c r="E73" s="72">
-        <f t="shared" ref="E73:E104" si="1">H73+21</f>
+      <c r="E73" s="6">
         <v>102193</v>
       </c>
       <c r="F73" s="8">
         <v>87231</v>
       </c>
       <c r="G73" s="8"/>
-      <c r="H73" s="8">
-        <v>102172</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="8"/>
+      <c r="J73" s="72"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>43934</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C74" s="8">
         <v>55391</v>
@@ -12220,19 +12430,17 @@
         <f t="shared" si="0"/>
         <v>1567</v>
       </c>
-      <c r="E74" s="72">
-        <f t="shared" si="1"/>
+      <c r="E74" s="6">
         <v>103554</v>
       </c>
       <c r="F74" s="8">
         <v>87616</v>
       </c>
       <c r="G74" s="8"/>
-      <c r="H74" s="8">
-        <v>103533</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H74" s="8"/>
+      <c r="J74" s="72"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>43935</v>
       </c>
@@ -12246,24 +12454,22 @@
         <f t="shared" si="0"/>
         <v>3648</v>
       </c>
-      <c r="E75" s="72">
-        <f t="shared" si="1"/>
+      <c r="E75" s="6">
         <v>104227</v>
       </c>
       <c r="F75" s="8">
         <v>88301</v>
       </c>
       <c r="G75" s="8"/>
-      <c r="H75" s="8">
-        <v>104206</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H75" s="8"/>
+      <c r="J75" s="72"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>43936</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C76" s="8">
         <v>58084</v>
@@ -12272,19 +12478,17 @@
         <f t="shared" si="0"/>
         <v>-955</v>
       </c>
-      <c r="E76" s="72">
-        <f t="shared" si="1"/>
+      <c r="E76" s="6">
         <v>105352</v>
       </c>
       <c r="F76" s="8">
         <v>90994</v>
       </c>
       <c r="G76" s="8"/>
-      <c r="H76" s="8">
-        <v>105331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H76" s="8"/>
+      <c r="J76" s="72"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>43937</v>
       </c>
@@ -12298,24 +12502,22 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="E77" s="72">
-        <f t="shared" si="1"/>
+      <c r="E77" s="6">
         <v>106538</v>
       </c>
       <c r="F77" s="8">
         <v>91021</v>
       </c>
       <c r="G77" s="8"/>
-      <c r="H77" s="8">
-        <v>106517</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H77" s="8"/>
+      <c r="J77" s="72"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>43938</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C78" s="8">
         <v>56151</v>
@@ -12324,24 +12526,22 @@
         <f t="shared" si="0"/>
         <v>-1964</v>
       </c>
-      <c r="E78" s="72">
-        <f t="shared" si="1"/>
+      <c r="E78" s="6">
         <v>106900</v>
       </c>
       <c r="F78" s="8">
         <v>96564</v>
       </c>
       <c r="G78" s="8"/>
-      <c r="H78" s="8">
-        <v>106879</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H78" s="8"/>
+      <c r="J78" s="72"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>43939</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C79" s="8">
         <v>56515</v>
@@ -12350,24 +12550,22 @@
         <f t="shared" si="0"/>
         <v>364</v>
       </c>
-      <c r="E79" s="72">
-        <f t="shared" si="1"/>
+      <c r="E79" s="6">
         <v>107704</v>
       </c>
       <c r="F79" s="8">
         <v>98382</v>
       </c>
       <c r="G79" s="8"/>
-      <c r="H79" s="8">
-        <v>107683</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H79" s="8"/>
+      <c r="J79" s="72"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>43940</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C80" s="8">
         <v>56310</v>
@@ -12376,198 +12574,182 @@
         <f t="shared" si="0"/>
         <v>-205</v>
       </c>
-      <c r="E80" s="72">
-        <f t="shared" si="1"/>
+      <c r="E80" s="6">
         <v>108186</v>
       </c>
       <c r="F80" s="8">
         <v>98338</v>
       </c>
       <c r="G80" s="8"/>
-      <c r="H80" s="8">
-        <v>108165</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H80" s="8"/>
+      <c r="J80" s="72"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>43941</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C81" s="8">
         <v>56983</v>
       </c>
       <c r="D81" s="25">
-        <f t="shared" ref="D81:D144" si="2">IFERROR(IFERROR(IFERROR(C81-C80,C81-C79),C81-C78),0)</f>
+        <f t="shared" ref="D81:D144" si="1">IFERROR(IFERROR(IFERROR(C81-C80,C81-C79),C81-C78),0)</f>
         <v>673</v>
       </c>
-      <c r="E81" s="72">
-        <f t="shared" si="1"/>
+      <c r="E81" s="6">
         <v>108158</v>
       </c>
       <c r="F81" s="8">
         <v>97464</v>
       </c>
       <c r="G81" s="8"/>
-      <c r="H81" s="8">
-        <v>108137</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H81" s="8"/>
+      <c r="J81" s="72"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>43942</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C82" s="8">
         <v>57347</v>
       </c>
       <c r="D82" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>364</v>
       </c>
-      <c r="E82" s="72">
-        <f t="shared" si="1"/>
+      <c r="E82" s="6">
         <v>107622</v>
       </c>
       <c r="F82" s="8">
         <v>98958</v>
       </c>
       <c r="G82" s="8"/>
-      <c r="H82" s="8">
-        <v>107601</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="8"/>
+      <c r="J82" s="72"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>43943</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C83" s="8">
         <v>57154</v>
       </c>
       <c r="D83" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-193</v>
       </c>
-      <c r="E83" s="72">
-        <f t="shared" si="1"/>
+      <c r="E83" s="6">
         <v>107606</v>
       </c>
       <c r="F83" s="8">
         <v>99440</v>
       </c>
       <c r="G83" s="8"/>
-      <c r="H83" s="8">
-        <v>107585</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="8"/>
+      <c r="J83" s="72"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>43944</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C84" s="8">
         <v>56860</v>
       </c>
       <c r="D84" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-294</v>
       </c>
-      <c r="E84" s="72">
-        <f t="shared" si="1"/>
+      <c r="E84" s="6">
         <v>106747</v>
       </c>
       <c r="F84" s="8">
         <v>100106</v>
       </c>
       <c r="G84" s="8"/>
-      <c r="H84" s="8">
-        <v>106726</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="8"/>
+      <c r="J84" s="72"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>43945</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C85" s="8">
         <v>56839</v>
       </c>
       <c r="D85" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-21</v>
       </c>
-      <c r="E85" s="72">
-        <f t="shared" si="1"/>
+      <c r="E85" s="6">
         <v>106421</v>
       </c>
       <c r="F85" s="8">
         <v>88111</v>
       </c>
-      <c r="H85" s="8">
-        <v>106400</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="8"/>
+      <c r="J85" s="72"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>43946</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C86" s="8">
         <v>56906</v>
       </c>
       <c r="D86" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="E86" s="72">
-        <f t="shared" si="1"/>
+      <c r="E86" s="6">
         <v>105736</v>
       </c>
       <c r="F86" s="8">
         <v>87295</v>
       </c>
-      <c r="H86" s="8">
-        <v>105715</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="8"/>
+      <c r="J86" s="72"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>43947</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C87" s="8">
         <v>56816</v>
       </c>
       <c r="D87" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-90</v>
       </c>
-      <c r="E87" s="72">
-        <f t="shared" si="1"/>
+      <c r="E87" s="6">
         <v>105989</v>
       </c>
       <c r="F87" s="8">
         <v>85712</v>
       </c>
-      <c r="H87" s="8">
-        <v>105968</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="8"/>
+      <c r="J87" s="72"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>43948</v>
       </c>
@@ -12578,196 +12760,180 @@
         <v>59533</v>
       </c>
       <c r="D88" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2717</v>
       </c>
-      <c r="E88" s="72">
-        <f t="shared" si="1"/>
+      <c r="E88" s="6">
         <v>105695</v>
       </c>
       <c r="F88" s="8">
         <v>85069</v>
       </c>
-      <c r="H88" s="8">
-        <v>105674</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="8"/>
+      <c r="J88" s="72"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>43949</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C89" s="8">
         <v>59313</v>
       </c>
       <c r="D89" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-220</v>
       </c>
-      <c r="E89" s="72">
-        <f t="shared" si="1"/>
+      <c r="E89" s="6">
         <v>105083</v>
       </c>
       <c r="F89" s="8">
         <v>84403</v>
       </c>
-      <c r="H89" s="8">
-        <v>105062</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="8"/>
+      <c r="J89" s="72"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>43950</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C90" s="8">
         <v>56127</v>
       </c>
       <c r="D90" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-3186</v>
       </c>
-      <c r="E90" s="72">
-        <f t="shared" si="1"/>
+      <c r="E90" s="6">
         <v>104530</v>
       </c>
       <c r="F90" s="8">
         <v>79695</v>
       </c>
-      <c r="H90" s="8">
-        <v>104509</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="8"/>
+      <c r="J90" s="72"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>43951</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C91" s="8">
         <v>55729</v>
       </c>
       <c r="D91" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-398</v>
       </c>
-      <c r="E91" s="72">
-        <f t="shared" si="1"/>
+      <c r="E91" s="6">
         <v>101414</v>
       </c>
       <c r="F91" s="8">
         <v>76842</v>
       </c>
-      <c r="H91" s="8">
-        <v>101393</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="8"/>
+      <c r="J91" s="72"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>43952</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C92" s="8">
         <v>55379</v>
       </c>
       <c r="D92" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-350</v>
       </c>
-      <c r="E92" s="72">
-        <f t="shared" si="1"/>
+      <c r="E92" s="6">
         <v>100801</v>
       </c>
       <c r="F92" s="8">
         <v>75714</v>
       </c>
-      <c r="H92" s="8">
-        <v>100780</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="8"/>
+      <c r="J92" s="72"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>43953</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C93" s="8">
         <v>55657</v>
       </c>
       <c r="D93" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
-      <c r="E93" s="72">
-        <f t="shared" si="1"/>
+      <c r="E93" s="6">
         <v>100559</v>
       </c>
       <c r="F93" s="8">
         <v>74234</v>
       </c>
-      <c r="H93" s="8">
-        <v>100538</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="8"/>
+      <c r="J93" s="72"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>43954</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C94" s="8">
         <v>55608</v>
       </c>
       <c r="D94" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-49</v>
       </c>
-      <c r="E94" s="72">
-        <f t="shared" si="1"/>
+      <c r="E94" s="6">
         <v>100030</v>
       </c>
       <c r="F94" s="8">
         <v>73300</v>
       </c>
-      <c r="H94" s="8">
-        <v>100009</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="8"/>
+      <c r="J94" s="72"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>43955</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C95" s="8">
         <v>55291</v>
       </c>
       <c r="D95" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-317</v>
       </c>
-      <c r="E95" s="72">
-        <f t="shared" si="1"/>
+      <c r="E95" s="6">
         <v>99829</v>
       </c>
       <c r="F95" s="8">
         <v>71240</v>
       </c>
-      <c r="H95" s="8">
-        <v>99808</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="8"/>
+      <c r="J95" s="72"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>43956</v>
       </c>
@@ -12778,96 +12944,88 @@
         <v>54700</v>
       </c>
       <c r="D96" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-591</v>
       </c>
-      <c r="E96" s="72">
-        <f t="shared" si="1"/>
+      <c r="E96" s="6">
         <v>98310</v>
       </c>
       <c r="F96" s="8">
         <v>70230</v>
       </c>
-      <c r="H96" s="8">
-        <v>98289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="8"/>
+      <c r="J96" s="72"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>43957</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C97" s="8">
         <v>57369</v>
       </c>
       <c r="D97" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2669</v>
       </c>
-      <c r="E97" s="72">
-        <f t="shared" si="1"/>
+      <c r="E97" s="6">
         <v>91354</v>
       </c>
       <c r="F97" s="8">
         <v>68466</v>
       </c>
-      <c r="H97" s="8">
-        <v>91333</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="8"/>
+      <c r="J97" s="72"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>43958</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C98" s="8">
         <v>56765</v>
       </c>
       <c r="D98" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-604</v>
       </c>
-      <c r="E98" s="72">
-        <f t="shared" si="1"/>
+      <c r="E98" s="6">
         <v>89444</v>
       </c>
       <c r="F98" s="8">
         <v>66866</v>
       </c>
-      <c r="H98" s="8">
-        <v>89423</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="8"/>
+      <c r="J98" s="72"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>43959</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" s="8">
         <v>56409</v>
       </c>
       <c r="D99" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-356</v>
       </c>
-      <c r="E99" s="72">
-        <f t="shared" si="1"/>
+      <c r="E99" s="6">
         <v>87775</v>
       </c>
       <c r="F99" s="8">
         <v>65410</v>
       </c>
-      <c r="H99" s="8">
-        <v>87754</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="8"/>
+      <c r="J99" s="72"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>43960</v>
       </c>
@@ -12878,46 +13036,42 @@
         <v>56506</v>
       </c>
       <c r="D100" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="E100" s="72">
-        <f t="shared" si="1"/>
+      <c r="E100" s="6">
         <v>84646</v>
       </c>
       <c r="F100" s="8">
         <v>63148</v>
       </c>
-      <c r="H100" s="8">
-        <v>84625</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H100" s="8"/>
+      <c r="J100" s="72"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>43961</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C101" s="8">
         <v>56466</v>
       </c>
       <c r="D101" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-40</v>
       </c>
-      <c r="E101" s="72">
-        <f t="shared" si="1"/>
+      <c r="E101" s="6">
         <v>83123</v>
       </c>
       <c r="F101" s="8">
         <v>61603</v>
       </c>
-      <c r="H101" s="8">
-        <v>83102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="8"/>
+      <c r="J101" s="72"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>43962</v>
       </c>
@@ -12928,46 +13082,42 @@
         <v>56152</v>
       </c>
       <c r="D102" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-314</v>
       </c>
-      <c r="E102" s="72">
-        <f t="shared" si="1"/>
+      <c r="E102" s="6">
         <v>82285</v>
       </c>
       <c r="F102" s="8">
         <v>63553</v>
       </c>
-      <c r="H102" s="8">
-        <v>82264</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H102" s="8"/>
+      <c r="J102" s="72"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>43963</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C103" s="8">
         <v>55451</v>
       </c>
       <c r="D103" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-701</v>
       </c>
-      <c r="E103" s="72">
-        <f t="shared" si="1"/>
+      <c r="E103" s="6">
         <v>81058</v>
       </c>
       <c r="F103" s="8">
         <v>62194</v>
       </c>
-      <c r="H103" s="8">
-        <v>81037</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H103" s="8"/>
+      <c r="J103" s="72"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>43964</v>
       </c>
@@ -12978,96 +13128,88 @@
         <v>54987</v>
       </c>
       <c r="D104" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-464</v>
       </c>
-      <c r="E104" s="72">
-        <f t="shared" si="1"/>
+      <c r="E104" s="6">
         <v>78241</v>
       </c>
       <c r="F104" s="8">
         <v>60902</v>
       </c>
-      <c r="H104" s="8">
-        <v>78220</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="8"/>
+      <c r="J104" s="72"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>43965</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C105" s="8">
         <v>54326</v>
       </c>
       <c r="D105" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-661</v>
       </c>
-      <c r="E105" s="72">
-        <f t="shared" ref="E105:E136" si="3">H105+21</f>
+      <c r="E105" s="6">
         <v>76218</v>
       </c>
       <c r="F105" s="8">
         <v>59068</v>
       </c>
-      <c r="H105" s="8">
-        <v>76197</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H105" s="8"/>
+      <c r="J105" s="72"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>43966</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C106" s="8">
         <v>53942</v>
       </c>
       <c r="D106" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-384</v>
       </c>
-      <c r="E106" s="72">
-        <f t="shared" si="3"/>
+      <c r="E106" s="6">
         <v>71836</v>
       </c>
       <c r="F106" s="8">
         <v>58206</v>
       </c>
-      <c r="H106" s="8">
-        <v>71815</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H106" s="8"/>
+      <c r="J106" s="72"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>43967</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C107" s="8">
         <v>53600</v>
       </c>
       <c r="D107" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-342</v>
       </c>
-      <c r="E107" s="72">
-        <f t="shared" si="3"/>
+      <c r="E107" s="6">
         <v>69947</v>
       </c>
       <c r="F107" s="8">
         <v>56996</v>
       </c>
-      <c r="H107" s="8">
-        <v>69926</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H107" s="8"/>
+      <c r="J107" s="72"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>43968</v>
       </c>
@@ -13078,72 +13220,66 @@
         <v>53090</v>
       </c>
       <c r="D108" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-510</v>
       </c>
-      <c r="E108" s="72">
-        <f t="shared" si="3"/>
+      <c r="E108" s="6">
         <v>68105</v>
       </c>
       <c r="F108" s="8">
         <v>54466</v>
       </c>
-      <c r="H108" s="8">
-        <v>68084</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H108" s="8"/>
+      <c r="J108" s="72"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>43969</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C109" s="8">
         <v>52936</v>
       </c>
       <c r="D109" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-154</v>
       </c>
-      <c r="E109" s="72">
-        <f t="shared" si="3"/>
+      <c r="E109" s="6">
         <v>66302</v>
       </c>
       <c r="F109" s="8">
         <v>53887</v>
       </c>
       <c r="G109" s="7"/>
-      <c r="H109" s="8">
-        <v>66281</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H109" s="8"/>
+      <c r="J109" s="72"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <v>43970</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C110" s="8">
         <v>52842</v>
       </c>
       <c r="D110" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-94</v>
       </c>
-      <c r="E110" s="72">
-        <f t="shared" si="3"/>
+      <c r="E110" s="6">
         <v>64873</v>
       </c>
       <c r="F110" s="8">
         <v>54461</v>
       </c>
-      <c r="H110" s="8">
-        <v>64852</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="8"/>
+      <c r="J110" s="72"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <v>43971</v>
       </c>
@@ -13154,71 +13290,65 @@
         <v>52359</v>
       </c>
       <c r="D111" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-483</v>
       </c>
-      <c r="E111" s="72">
-        <f t="shared" si="3"/>
+      <c r="E111" s="6">
         <v>62489</v>
       </c>
       <c r="F111" s="8">
         <v>55116</v>
       </c>
-      <c r="H111" s="8">
-        <v>62468</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H111" s="8"/>
+      <c r="J111" s="72"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>43972</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C112" s="8">
         <v>52090</v>
       </c>
       <c r="D112" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-269</v>
       </c>
-      <c r="E112" s="72">
-        <f t="shared" si="3"/>
+      <c r="E112" s="6">
         <v>60692</v>
       </c>
       <c r="F112" s="8">
         <v>55657</v>
       </c>
-      <c r="H112" s="8">
-        <v>60671</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H112" s="8"/>
+      <c r="J112" s="72"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>43973</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C113" s="8">
         <v>52058</v>
       </c>
       <c r="D113" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-32</v>
       </c>
-      <c r="E113" s="72">
-        <f t="shared" si="3"/>
+      <c r="E113" s="6">
         <v>59050</v>
       </c>
       <c r="F113" s="8">
         <v>57374</v>
       </c>
-      <c r="H113" s="8">
-        <v>59029</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H113" s="8"/>
+      <c r="J113" s="72"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <v>43974</v>
       </c>
@@ -13229,21 +13359,19 @@
         <v>51927</v>
       </c>
       <c r="D114" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-131</v>
       </c>
-      <c r="E114" s="72">
-        <f t="shared" si="3"/>
+      <c r="E114" s="6">
         <v>57476</v>
       </c>
       <c r="F114" s="8">
         <v>57790</v>
       </c>
-      <c r="H114" s="8">
-        <v>57455</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H114" s="8"/>
+      <c r="J114" s="72"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <v>43975</v>
       </c>
@@ -13254,71 +13382,65 @@
         <v>51937</v>
       </c>
       <c r="D115" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E115" s="72">
-        <f t="shared" si="3"/>
+      <c r="E115" s="6">
         <v>56315</v>
       </c>
       <c r="F115" s="8">
         <v>58198</v>
       </c>
-      <c r="H115" s="8">
-        <v>56294</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H115" s="8"/>
+      <c r="J115" s="72"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <v>43976</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C116" s="8">
         <v>51648</v>
       </c>
       <c r="D116" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-289</v>
       </c>
-      <c r="E116" s="72">
-        <f t="shared" si="3"/>
+      <c r="E116" s="6">
         <v>55017</v>
       </c>
       <c r="F116" s="8">
         <v>57754</v>
       </c>
-      <c r="H116" s="8">
-        <v>54996</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H116" s="8"/>
+      <c r="J116" s="72"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>43977</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C117" s="8">
         <v>51146</v>
       </c>
       <c r="D117" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-502</v>
       </c>
-      <c r="E117" s="72">
-        <f t="shared" si="3"/>
+      <c r="E117" s="6">
         <v>52653</v>
       </c>
       <c r="F117" s="8">
         <v>58538</v>
       </c>
-      <c r="H117" s="8">
-        <v>52632</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H117" s="8"/>
+      <c r="J117" s="72"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>43978</v>
       </c>
@@ -13329,71 +13451,65 @@
         <v>50566</v>
       </c>
       <c r="D118" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-580</v>
       </c>
-      <c r="E118" s="72">
-        <f t="shared" si="3"/>
+      <c r="E118" s="6">
         <v>50672</v>
       </c>
       <c r="F118" s="8">
         <v>59006</v>
       </c>
-      <c r="H118" s="8">
-        <v>50651</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H118" s="8"/>
+      <c r="J118" s="72"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>43979</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C119" s="8">
         <v>53218</v>
       </c>
       <c r="D119" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2652</v>
       </c>
-      <c r="E119" s="72">
-        <f t="shared" si="3"/>
+      <c r="E119" s="6">
         <v>47682</v>
       </c>
       <c r="F119" s="8">
         <v>60106</v>
       </c>
-      <c r="H119" s="8">
-        <v>47661</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H119" s="8"/>
+      <c r="J119" s="72"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>43980</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C120" s="8">
         <v>53151</v>
       </c>
       <c r="D120" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-67</v>
       </c>
-      <c r="E120" s="72">
-        <f t="shared" si="3"/>
+      <c r="E120" s="6">
         <v>45867</v>
       </c>
       <c r="F120" s="8">
         <v>60734</v>
       </c>
-      <c r="H120" s="8">
-        <v>45846</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H120" s="8"/>
+      <c r="J120" s="72"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>43981</v>
       </c>
@@ -13404,21 +13520,19 @@
         <v>54457</v>
       </c>
       <c r="D121" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1306</v>
       </c>
-      <c r="E121" s="72">
-        <f t="shared" si="3"/>
+      <c r="E121" s="6">
         <v>43377</v>
       </c>
       <c r="F121" s="8">
         <v>61360</v>
       </c>
-      <c r="H121" s="8">
-        <v>43356</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H121" s="8"/>
+      <c r="J121" s="72"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <v>43982</v>
       </c>
@@ -13429,21 +13543,19 @@
         <v>54596</v>
       </c>
       <c r="D122" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
-      <c r="E122" s="72">
-        <f t="shared" si="3"/>
+      <c r="E122" s="6">
         <v>41757</v>
       </c>
       <c r="F122" s="8">
         <v>61521</v>
       </c>
-      <c r="H122" s="8">
-        <v>41736</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H122" s="8"/>
+      <c r="J122" s="72"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <v>43983</v>
       </c>
@@ -13454,21 +13566,19 @@
         <v>54818</v>
       </c>
       <c r="D123" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>222</v>
       </c>
-      <c r="E123" s="72">
-        <f t="shared" si="3"/>
+      <c r="E123" s="6">
         <v>41047</v>
       </c>
       <c r="F123" s="8">
         <v>61702</v>
       </c>
-      <c r="H123" s="8">
-        <v>41026</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H123" s="8"/>
+      <c r="J123" s="72"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <v>43984</v>
       </c>
@@ -13479,46 +13589,42 @@
         <v>53573</v>
       </c>
       <c r="D124" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1245</v>
       </c>
-      <c r="E124" s="72">
-        <f t="shared" si="3"/>
+      <c r="E124" s="6">
         <v>39570</v>
       </c>
       <c r="F124" s="8">
         <v>61976</v>
       </c>
-      <c r="H124" s="8">
-        <v>39549</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H124" s="8"/>
+      <c r="J124" s="72"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>43985</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C125" s="8">
         <v>53201</v>
       </c>
       <c r="D125" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-372</v>
       </c>
-      <c r="E125" s="72">
-        <f t="shared" si="3"/>
+      <c r="E125" s="6">
         <v>38973</v>
       </c>
       <c r="F125" s="8">
         <v>62340</v>
       </c>
-      <c r="H125" s="8">
-        <v>38952</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H125" s="8"/>
+      <c r="J125" s="72"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>43986</v>
       </c>
@@ -13529,246 +13635,226 @@
         <v>53403</v>
       </c>
       <c r="D126" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>202</v>
       </c>
-      <c r="E126" s="72">
-        <f t="shared" si="3"/>
+      <c r="E126" s="6">
         <v>38103</v>
       </c>
       <c r="F126" s="8">
         <v>62649</v>
       </c>
-      <c r="H126" s="8">
-        <v>38082</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H126" s="8"/>
+      <c r="J126" s="72"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>43987</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C127" s="8">
         <v>53440</v>
       </c>
       <c r="D127" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="E127" s="72">
-        <f t="shared" si="3"/>
+      <c r="E127" s="6">
         <v>36646</v>
       </c>
       <c r="F127" s="8">
         <v>62937</v>
       </c>
-      <c r="H127" s="8">
-        <v>36625</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H127" s="8"/>
+      <c r="J127" s="72"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>43988</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C128" s="8">
         <v>53686</v>
       </c>
       <c r="D128" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
-      <c r="E128" s="72">
-        <f t="shared" si="3"/>
+      <c r="E128" s="6">
         <v>35544</v>
       </c>
       <c r="F128" s="8">
         <v>63254</v>
       </c>
-      <c r="H128" s="8">
-        <v>35523</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H128" s="8"/>
+      <c r="J128" s="72"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>43989</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C129" s="8">
         <v>53980</v>
       </c>
       <c r="D129" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
-      <c r="E129" s="72">
-        <f t="shared" si="3"/>
+      <c r="E129" s="6">
         <v>34927</v>
       </c>
       <c r="F129" s="8">
         <v>63475</v>
       </c>
-      <c r="H129" s="8">
-        <v>34906</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H129" s="8"/>
+      <c r="J129" s="72"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>43990</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C130" s="8">
         <v>53917</v>
       </c>
       <c r="D130" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-63</v>
       </c>
-      <c r="E130" s="72">
-        <f t="shared" si="3"/>
+      <c r="E130" s="6">
         <v>34393</v>
       </c>
       <c r="F130" s="8">
         <v>63630</v>
       </c>
-      <c r="H130" s="8">
-        <v>34372</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H130" s="8"/>
+      <c r="J130" s="72"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <v>43991</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C131" s="8">
         <v>53789</v>
       </c>
       <c r="D131" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-128</v>
       </c>
-      <c r="E131" s="72">
-        <f t="shared" si="3"/>
+      <c r="E131" s="6">
         <v>32530</v>
       </c>
       <c r="F131" s="8">
         <v>63862</v>
       </c>
-      <c r="H131" s="8">
-        <v>32509</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H131" s="8"/>
+      <c r="J131" s="72"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>43992</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C132" s="8">
         <v>53985</v>
       </c>
       <c r="D132" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="E132" s="72">
-        <f t="shared" si="3"/>
+      <c r="E132" s="6">
         <v>31365</v>
       </c>
       <c r="F132" s="8">
         <v>64166</v>
       </c>
-      <c r="H132" s="8">
-        <v>31344</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H132" s="8"/>
+      <c r="J132" s="72"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <v>43993</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C133" s="8">
         <v>54066</v>
       </c>
       <c r="D133" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="E133" s="72">
-        <f t="shared" si="3"/>
+      <c r="E133" s="6">
         <v>30290</v>
       </c>
       <c r="F133" s="8">
         <v>64570</v>
       </c>
-      <c r="H133" s="8">
-        <v>30269</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H133" s="8"/>
+      <c r="J133" s="72"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>43994</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C134" s="8">
         <v>54341</v>
       </c>
       <c r="D134" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>275</v>
       </c>
-      <c r="E134" s="72">
-        <f t="shared" si="3"/>
+      <c r="E134" s="6">
         <v>28646</v>
       </c>
       <c r="F134" s="8">
         <v>65056</v>
       </c>
-      <c r="H134" s="8">
-        <v>28625</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H134" s="8"/>
+      <c r="J134" s="72"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <v>43995</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C135" s="8">
         <v>54607</v>
       </c>
       <c r="D135" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>266</v>
       </c>
-      <c r="E135" s="72">
-        <f t="shared" si="3"/>
+      <c r="E135" s="6">
         <v>27131</v>
       </c>
       <c r="F135" s="8">
         <v>65443</v>
       </c>
-      <c r="H135" s="8">
-        <v>27110</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H135" s="8"/>
+      <c r="J135" s="72"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <v>43996</v>
       </c>
@@ -13779,371 +13865,341 @@
         <v>54954</v>
       </c>
       <c r="D136" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>347</v>
       </c>
-      <c r="E136" s="72">
-        <f t="shared" si="3"/>
+      <c r="E136" s="6">
         <v>25915</v>
       </c>
       <c r="F136" s="8">
         <v>65759</v>
       </c>
-      <c r="H136" s="8">
-        <v>25894</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H136" s="8"/>
+      <c r="J136" s="72"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <v>43997</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C137" s="8">
         <v>54892</v>
       </c>
       <c r="D137" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-62</v>
       </c>
-      <c r="E137" s="72">
-        <f t="shared" ref="E137:E168" si="4">H137+21</f>
+      <c r="E137" s="6">
         <v>25548</v>
       </c>
       <c r="F137" s="8">
         <v>65932</v>
       </c>
-      <c r="H137" s="8">
-        <v>25527</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H137" s="8"/>
+      <c r="J137" s="72"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <v>43998</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C138" s="8">
         <v>54834</v>
       </c>
       <c r="D138" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-58</v>
       </c>
-      <c r="E138" s="72">
-        <f t="shared" si="4"/>
+      <c r="E138" s="6">
         <v>24204</v>
       </c>
       <c r="F138" s="8">
         <v>66144</v>
       </c>
-      <c r="H138" s="8">
-        <v>24183</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H138" s="8"/>
+      <c r="J138" s="72"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <v>43999</v>
       </c>
       <c r="B139" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C139" s="8">
         <v>54932</v>
       </c>
       <c r="D139" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="E139" s="72">
-        <f t="shared" si="4"/>
+      <c r="E139" s="6">
         <v>23559</v>
       </c>
       <c r="F139" s="8">
         <v>66493</v>
       </c>
-      <c r="H139" s="8">
-        <v>23538</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H139" s="8"/>
+      <c r="J139" s="72"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>44000</v>
       </c>
       <c r="B140" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C140" s="8">
         <v>55151</v>
       </c>
       <c r="D140" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>219</v>
       </c>
-      <c r="E140" s="72">
-        <f t="shared" si="4"/>
+      <c r="E140" s="6">
         <v>22733</v>
       </c>
       <c r="F140" s="8">
         <v>67075</v>
       </c>
-      <c r="H140" s="8">
-        <v>22712</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H140" s="8"/>
+      <c r="J140" s="72"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>44001</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C141" s="8">
         <v>55718</v>
       </c>
       <c r="D141" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>567</v>
       </c>
-      <c r="E141" s="72">
-        <f t="shared" si="4"/>
+      <c r="E141" s="6">
         <v>21571</v>
       </c>
       <c r="F141" s="8">
         <v>67382</v>
       </c>
-      <c r="H141" s="8">
-        <v>21550</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H141" s="8"/>
+      <c r="J141" s="72"/>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>44002</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C142" s="8">
         <v>56148</v>
       </c>
       <c r="D142" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>430</v>
       </c>
-      <c r="E142" s="72">
-        <f t="shared" si="4"/>
+      <c r="E142" s="6">
         <v>21239</v>
       </c>
       <c r="F142" s="8">
         <v>67738</v>
       </c>
-      <c r="H142" s="8">
-        <v>21218</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H142" s="8"/>
+      <c r="J142" s="72"/>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <v>44003</v>
       </c>
       <c r="B143" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C143" s="8">
         <v>56365</v>
       </c>
       <c r="D143" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>217</v>
       </c>
-      <c r="E143" s="72">
-        <f t="shared" si="4"/>
+      <c r="E143" s="6">
         <v>20998</v>
       </c>
       <c r="F143" s="8">
         <v>68071</v>
       </c>
-      <c r="H143" s="8">
-        <v>20977</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H143" s="8"/>
+      <c r="J143" s="72"/>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <v>44004</v>
       </c>
       <c r="B144" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C144" s="8">
         <v>56475</v>
       </c>
       <c r="D144" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="E144" s="72">
-        <f t="shared" si="4"/>
+      <c r="E144" s="6">
         <v>20662</v>
       </c>
       <c r="F144" s="8">
         <v>68302</v>
       </c>
-      <c r="H144" s="8">
-        <v>20641</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H144" s="8"/>
+      <c r="J144" s="72"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>44005</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C145" s="8">
         <v>56676</v>
       </c>
       <c r="D145" s="25">
-        <f t="shared" ref="D145:D181" si="5">IFERROR(IFERROR(IFERROR(C145-C144,C145-C143),C145-C142),0)</f>
+        <f t="shared" ref="D145:D190" si="2">IFERROR(IFERROR(IFERROR(C145-C144,C145-C143),C145-C142),0)</f>
         <v>201</v>
       </c>
-      <c r="E145" s="72">
-        <f t="shared" si="4"/>
+      <c r="E145" s="6">
         <v>19595</v>
       </c>
       <c r="F145" s="8">
         <v>68549</v>
       </c>
-      <c r="H145" s="8">
-        <v>19574</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H145" s="8"/>
+      <c r="J145" s="72"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="9">
         <v>44006</v>
       </c>
       <c r="B146" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C146" s="8">
         <v>56490</v>
       </c>
       <c r="D146" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-186</v>
       </c>
-      <c r="E146" s="72">
-        <f t="shared" si="4"/>
+      <c r="E146" s="6">
         <v>18676</v>
       </c>
       <c r="F146" s="8">
         <v>68881</v>
       </c>
-      <c r="H146" s="8">
-        <v>18655</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H146" s="8"/>
+      <c r="J146" s="72"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>44007</v>
       </c>
       <c r="B147" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C147" s="8">
         <v>56245</v>
       </c>
       <c r="D147" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>-245</v>
       </c>
-      <c r="E147" s="72">
-        <f t="shared" si="4"/>
+      <c r="E147" s="6">
         <v>18324</v>
       </c>
       <c r="F147" s="8">
         <v>69278</v>
       </c>
-      <c r="H147" s="8">
-        <v>18303</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H147" s="8"/>
+      <c r="J147" s="72"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <v>44008</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C148" s="68">
         <v>57509</v>
       </c>
       <c r="D148" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1264</v>
       </c>
-      <c r="E148" s="72">
-        <f t="shared" si="4"/>
+      <c r="E148" s="6">
         <v>17659</v>
       </c>
       <c r="F148" s="8">
         <v>69689</v>
       </c>
-      <c r="H148" s="8">
-        <v>17638</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H148" s="8"/>
+      <c r="J148" s="72"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="9">
         <v>44009</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C149" s="69" t="s">
         <v>76</v>
       </c>
       <c r="D149" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E149" s="72">
-        <f t="shared" si="4"/>
+      <c r="E149" s="6">
         <v>16857</v>
       </c>
       <c r="F149" s="8">
         <v>70250</v>
       </c>
-      <c r="H149" s="8">
-        <v>16836</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H149" s="8"/>
+      <c r="J149" s="72"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="9">
         <v>44010</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C150" s="69" t="s">
         <v>76</v>
       </c>
       <c r="D150" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E150" s="72">
-        <f t="shared" si="4"/>
+      <c r="E150" s="6">
         <v>16702</v>
       </c>
       <c r="F150" s="8">
         <v>70549</v>
       </c>
-      <c r="H150" s="8">
-        <v>16681</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H150" s="8"/>
+      <c r="J150" s="72"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="9">
         <v>44011</v>
       </c>
@@ -14154,46 +14210,42 @@
         <v>58448</v>
       </c>
       <c r="D151" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>939</v>
       </c>
-      <c r="E151" s="72">
-        <f t="shared" si="4"/>
+      <c r="E151" s="6">
         <v>16517</v>
       </c>
       <c r="F151" s="8">
         <v>70746</v>
       </c>
-      <c r="H151" s="8">
-        <v>16496</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H151" s="8"/>
+      <c r="J151" s="72"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="9">
         <v>44012</v>
       </c>
       <c r="B152" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C152" s="8">
         <v>58684</v>
       </c>
       <c r="D152" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>236</v>
       </c>
-      <c r="E152" s="72">
-        <f t="shared" si="4"/>
+      <c r="E152" s="6">
         <v>15584</v>
       </c>
       <c r="F152" s="8">
         <v>71038</v>
       </c>
-      <c r="H152" s="8">
-        <v>15563</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H152" s="8"/>
+      <c r="J152" s="72"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <v>44013</v>
       </c>
@@ -14204,21 +14256,19 @@
         <v>59319</v>
       </c>
       <c r="D153" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>635</v>
       </c>
-      <c r="E153" s="72">
-        <f t="shared" si="4"/>
+      <c r="E153" s="6">
         <v>15276</v>
       </c>
       <c r="F153" s="8">
         <v>71418</v>
       </c>
-      <c r="H153" s="8">
-        <v>15255</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H153" s="8"/>
+      <c r="J153" s="72"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <v>44014</v>
       </c>
@@ -14229,21 +14279,19 @@
         <v>59701</v>
       </c>
       <c r="D154" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>382</v>
       </c>
-      <c r="E154" s="72">
-        <f t="shared" si="4"/>
+      <c r="E154" s="6">
         <v>15081</v>
       </c>
       <c r="F154" s="6">
         <v>71857</v>
       </c>
-      <c r="H154" s="6">
-        <v>15060</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H154" s="6"/>
+      <c r="J154" s="72"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="9">
         <v>44015</v>
       </c>
@@ -14254,21 +14302,19 @@
         <v>60007</v>
       </c>
       <c r="D155" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>306</v>
       </c>
-      <c r="E155" s="72">
-        <f t="shared" si="4"/>
+      <c r="E155" s="6">
         <v>14905</v>
       </c>
       <c r="F155" s="6">
         <v>72282</v>
       </c>
-      <c r="H155" s="6">
-        <v>14884</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H155" s="6"/>
+      <c r="J155" s="72"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <v>44016</v>
       </c>
@@ -14279,21 +14325,19 @@
         <v>76</v>
       </c>
       <c r="D156" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E156" s="72">
-        <f t="shared" si="4"/>
+      <c r="E156" s="6">
         <v>14642</v>
       </c>
       <c r="F156" s="6">
         <v>72697</v>
       </c>
-      <c r="H156" s="6">
-        <v>14621</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H156" s="6"/>
+      <c r="J156" s="72"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <v>44017</v>
       </c>
@@ -14304,21 +14348,19 @@
         <v>76</v>
       </c>
       <c r="D157" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E157" s="72">
-        <f t="shared" si="4"/>
+      <c r="E157" s="6">
         <v>14663</v>
       </c>
       <c r="F157" s="6">
         <v>73112</v>
       </c>
-      <c r="H157" s="6">
-        <v>14642</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H157" s="6"/>
+      <c r="J157" s="72"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <v>44018</v>
       </c>
@@ -14329,21 +14371,19 @@
         <v>61096</v>
       </c>
       <c r="D158" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1089</v>
       </c>
-      <c r="E158" s="72">
-        <f t="shared" si="4"/>
+      <c r="E158" s="6">
         <v>14730</v>
       </c>
       <c r="F158" s="6">
         <v>73523</v>
       </c>
-      <c r="H158" s="6">
-        <v>14709</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H158" s="6"/>
+      <c r="J158" s="72"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <v>44019</v>
       </c>
@@ -14354,21 +14394,19 @@
         <v>61222</v>
       </c>
       <c r="D159" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
-      <c r="E159" s="72">
-        <f t="shared" si="4"/>
+      <c r="E159" s="6">
         <v>14263</v>
       </c>
       <c r="F159" s="6">
         <v>73860</v>
       </c>
-      <c r="H159" s="6">
-        <v>14242</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H159" s="6"/>
+      <c r="J159" s="72"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="9">
         <v>44020</v>
       </c>
@@ -14379,21 +14417,19 @@
         <v>61512</v>
       </c>
       <c r="D160" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>290</v>
       </c>
-      <c r="E160" s="72">
-        <f t="shared" si="4"/>
+      <c r="E160" s="6">
         <v>13616</v>
       </c>
       <c r="F160" s="6">
         <v>74239</v>
       </c>
-      <c r="H160" s="6">
-        <v>13595</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H160" s="6"/>
+      <c r="J160" s="72"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="9">
         <v>44021</v>
       </c>
@@ -14404,46 +14440,42 @@
         <v>61945</v>
       </c>
       <c r="D161" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>433</v>
       </c>
-      <c r="E161" s="72">
-        <f t="shared" si="4"/>
+      <c r="E161" s="6">
         <v>13480</v>
       </c>
       <c r="F161" s="6">
         <v>74777</v>
       </c>
-      <c r="H161" s="6">
-        <v>13459</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H161" s="6"/>
+      <c r="J161" s="72"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="9">
         <v>44022</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C162" s="6">
         <v>62360</v>
       </c>
       <c r="D162" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>415</v>
       </c>
-      <c r="E162" s="72">
-        <f t="shared" si="4"/>
+      <c r="E162" s="6">
         <v>13449</v>
       </c>
       <c r="F162" s="6">
         <v>75627</v>
       </c>
-      <c r="H162" s="6">
-        <v>13428</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H162" s="6"/>
+      <c r="J162" s="72"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="9">
         <v>44023</v>
       </c>
@@ -14454,21 +14486,19 @@
         <v>76</v>
       </c>
       <c r="D163" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E163" s="72">
-        <f t="shared" si="4"/>
+      <c r="E163" s="6">
         <v>13324</v>
       </c>
       <c r="F163" s="6">
         <v>76308</v>
       </c>
-      <c r="H163" s="6">
-        <v>13303</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H163" s="6"/>
+      <c r="J163" s="72"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="9">
         <v>44024</v>
       </c>
@@ -14479,21 +14509,19 @@
         <v>76</v>
       </c>
       <c r="D164" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E164" s="72">
-        <f t="shared" si="4"/>
+      <c r="E164" s="6">
         <v>13200</v>
       </c>
       <c r="F164" s="6">
         <v>76989</v>
       </c>
-      <c r="H164" s="6">
-        <v>13179</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H164" s="6"/>
+      <c r="J164" s="72"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="9">
         <v>44025</v>
       </c>
@@ -14504,21 +14532,19 @@
         <v>63751</v>
       </c>
       <c r="D165" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1391</v>
       </c>
-      <c r="E165" s="72">
-        <f t="shared" si="4"/>
+      <c r="E165" s="6">
         <v>13178</v>
       </c>
       <c r="F165" s="6">
         <v>77669</v>
       </c>
-      <c r="H165" s="6">
-        <v>13157</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H165" s="6"/>
+      <c r="J165" s="72"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="9">
         <v>44026</v>
       </c>
@@ -14529,21 +14555,19 @@
         <v>76</v>
       </c>
       <c r="D166" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E166" s="72">
-        <f t="shared" si="4"/>
+      <c r="E166" s="6">
         <v>12940</v>
       </c>
       <c r="F166" s="6">
         <v>78332</v>
       </c>
-      <c r="H166" s="6">
-        <v>12919</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H166" s="6"/>
+      <c r="J166" s="72"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="9">
         <v>44027</v>
       </c>
@@ -14554,21 +14578,19 @@
         <v>64364</v>
       </c>
       <c r="D167" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>613</v>
       </c>
-      <c r="E167" s="72">
-        <f t="shared" si="4"/>
+      <c r="E167" s="6">
         <v>12514</v>
       </c>
       <c r="F167" s="6">
         <v>79203</v>
       </c>
-      <c r="H167" s="6">
-        <v>12493</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H167" s="6"/>
+      <c r="J167" s="72"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="9">
         <v>44028</v>
       </c>
@@ -14579,32 +14601,30 @@
         <v>64664</v>
       </c>
       <c r="D168" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="E168" s="72">
-        <f t="shared" si="4"/>
+      <c r="E168" s="6">
         <v>12494</v>
       </c>
       <c r="F168" s="6">
         <v>80561</v>
       </c>
-      <c r="H168" s="6">
-        <v>12473</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H168" s="6"/>
+      <c r="J168" s="72"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="9">
         <v>44029</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C169" s="6">
         <v>65278</v>
       </c>
       <c r="D169" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>614</v>
       </c>
       <c r="E169" s="6">
@@ -14614,18 +14634,18 @@
         <v>81957</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <v>44030</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C170" s="70" t="s">
         <v>76</v>
       </c>
       <c r="D170" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E170" s="6">
@@ -14635,18 +14655,18 @@
         <v>83484</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="9">
         <v>44031</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C171" s="70" t="s">
         <v>76</v>
       </c>
       <c r="D171" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E171" s="6">
@@ -14656,18 +14676,18 @@
         <v>85011</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="9">
         <v>44032</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C172" s="6">
         <v>67036</v>
       </c>
       <c r="D172" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1758</v>
       </c>
       <c r="E172" s="6">
@@ -14677,18 +14697,18 @@
         <v>86536</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="9">
         <v>44033</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C173" s="6">
         <v>67439</v>
       </c>
       <c r="D173" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>403</v>
       </c>
       <c r="E173" s="6">
@@ -14698,18 +14718,18 @@
         <v>87892</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="9">
         <v>44034</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C174" s="6">
         <v>68207</v>
       </c>
       <c r="D174" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>768</v>
       </c>
       <c r="E174" s="6">
@@ -14719,18 +14739,18 @@
         <v>89247</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="9">
         <v>44035</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C175" s="6">
         <v>68744</v>
       </c>
       <c r="D175" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>537</v>
       </c>
       <c r="E175" s="6">
@@ -14740,18 +14760,18 @@
         <v>91859</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="9">
         <v>44036</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C176" s="6">
         <v>69521</v>
       </c>
       <c r="D176" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>777</v>
       </c>
       <c r="E176" s="6">
@@ -14766,13 +14786,13 @@
         <v>44037</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C177" s="70" t="s">
         <v>76</v>
       </c>
       <c r="D177" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E177" s="6">
@@ -14787,13 +14807,13 @@
         <v>44038</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C178" s="70" t="s">
         <v>76</v>
       </c>
       <c r="D178" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E178" s="6">
@@ -14808,13 +14828,13 @@
         <v>44039</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C179" s="6">
         <v>71788</v>
       </c>
       <c r="D179" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2267</v>
       </c>
       <c r="E179" s="6">
@@ -14829,13 +14849,13 @@
         <v>44040</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C180" s="6">
         <v>72270</v>
       </c>
       <c r="D180" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>482</v>
       </c>
       <c r="E180" s="6">
@@ -14850,13 +14870,13 @@
         <v>44041</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C181" s="6">
         <v>73458</v>
       </c>
       <c r="D181" s="25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1188</v>
       </c>
       <c r="E181" s="6">
@@ -14871,9 +14891,15 @@
         <v>44042</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="D182" s="25"/>
+        <v>266</v>
+      </c>
+      <c r="C182" s="6">
+        <v>74652</v>
+      </c>
+      <c r="D182" s="25">
+        <f t="shared" si="2"/>
+        <v>1194</v>
+      </c>
       <c r="E182" s="6">
         <v>12230</v>
       </c>
@@ -14886,9 +14912,15 @@
         <v>44043</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="D183" s="25"/>
+        <v>267</v>
+      </c>
+      <c r="C183" s="6">
+        <v>75773</v>
+      </c>
+      <c r="D183" s="25">
+        <f t="shared" si="2"/>
+        <v>1121</v>
+      </c>
       <c r="E183" s="6">
         <v>12422</v>
       </c>
@@ -14896,8 +14928,155 @@
         <v>110199</v>
       </c>
     </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="9">
+        <v>44044</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C184" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D184" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E184" s="6">
+        <v>12457</v>
+      </c>
+      <c r="F184" s="6">
+        <v>112704</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="9">
+        <v>44045</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C185" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="D185" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E185" s="6">
+        <v>12456</v>
+      </c>
+      <c r="F185" s="6">
+        <v>115669</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="9">
+        <v>44046</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C186" s="6">
+        <v>78835</v>
+      </c>
+      <c r="D186" s="25">
+        <f t="shared" si="2"/>
+        <v>3062</v>
+      </c>
+      <c r="E186" s="6">
+        <v>12474</v>
+      </c>
+      <c r="F186" s="6">
+        <v>118704</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="9">
+        <v>44047</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C187" s="6">
+        <v>79720</v>
+      </c>
+      <c r="D187" s="25">
+        <f t="shared" si="2"/>
+        <v>885</v>
+      </c>
+      <c r="E187" s="6">
+        <v>12482</v>
+      </c>
+      <c r="F187" s="6">
+        <v>124438</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="9">
+        <v>44048</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C188" s="6">
+        <v>81264</v>
+      </c>
+      <c r="D188" s="25">
+        <f t="shared" si="2"/>
+        <v>1544</v>
+      </c>
+      <c r="E188" s="6">
+        <v>12646</v>
+      </c>
+      <c r="F188" s="6">
+        <v>127390</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="9">
+        <v>44049</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C189" s="6">
+        <v>82651</v>
+      </c>
+      <c r="D189" s="25">
+        <f t="shared" si="2"/>
+        <v>1387</v>
+      </c>
+      <c r="E189" s="6">
+        <v>12694</v>
+      </c>
+      <c r="F189" s="6">
+        <v>131477</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="9">
+        <v>44050</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C190" s="6">
+        <v>84761</v>
+      </c>
+      <c r="D190" s="25">
+        <f t="shared" si="2"/>
+        <v>2110</v>
+      </c>
+      <c r="E190" s="6">
+        <v>12924</v>
+      </c>
+      <c r="F190" s="6">
+        <v>135981</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D15:D181">
+  <conditionalFormatting sqref="D15:D190">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>IFERROR(IFERROR(-0.01*C14,-0.01*C13),-0.01*C12)</formula>
       <formula>IFERROR(IFERROR(0.01*C14,0.01*C13),0.01*C12)</formula>
@@ -15050,9 +15229,7 @@
       <c r="B14" s="44"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
-        <v>274</v>
-      </c>
+      <c r="A15" s="62"/>
       <c r="B15" s="59"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -15336,16 +15513,16 @@
         <v>44044</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="40" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="E17" s="37" t="s">
         <v>269</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -15353,16 +15530,16 @@
         <v>44044</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="37" t="s">
         <v>271</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -15379,7 +15556,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0051AC5D-FE47-43E6-8AF1-4AEA504DE4AE}">
-  <dimension ref="A1:N183"/>
+  <dimension ref="A1:N190"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -18468,7 +18645,7 @@
         <v>3300</v>
       </c>
       <c r="C133" s="25">
-        <f t="shared" ref="C133:C183" si="2">B133*1000</f>
+        <f t="shared" ref="C133:C190" si="2">B133*1000</f>
         <v>3300000</v>
       </c>
       <c r="D133" s="8">
@@ -19320,6 +19497,9 @@
         <f t="shared" si="2"/>
         <v>5856000</v>
       </c>
+      <c r="D182" s="6">
+        <v>74652</v>
+      </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="9">
@@ -19331,6 +19511,110 @@
       <c r="C183" s="6">
         <f t="shared" si="2"/>
         <v>5915000</v>
+      </c>
+      <c r="D183" s="6">
+        <v>75773</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="9">
+        <v>44044</v>
+      </c>
+      <c r="B184" s="6">
+        <v>5997</v>
+      </c>
+      <c r="C184" s="6">
+        <f t="shared" si="2"/>
+        <v>5997000</v>
+      </c>
+      <c r="D184" s="70"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="9">
+        <v>44045</v>
+      </c>
+      <c r="B185" s="6">
+        <v>6067</v>
+      </c>
+      <c r="C185" s="6">
+        <f t="shared" si="2"/>
+        <v>6067000</v>
+      </c>
+      <c r="D185" s="70"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="9">
+        <v>44046</v>
+      </c>
+      <c r="B186" s="6">
+        <v>6057</v>
+      </c>
+      <c r="C186" s="6">
+        <f t="shared" si="2"/>
+        <v>6057000</v>
+      </c>
+      <c r="D186" s="6">
+        <v>78835</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="9">
+        <v>44047</v>
+      </c>
+      <c r="B187" s="6">
+        <v>6074</v>
+      </c>
+      <c r="C187" s="6">
+        <f t="shared" si="2"/>
+        <v>6074000</v>
+      </c>
+      <c r="D187" s="6">
+        <v>79720</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="9">
+        <v>44048</v>
+      </c>
+      <c r="B188" s="6">
+        <v>6098</v>
+      </c>
+      <c r="C188" s="6">
+        <f t="shared" si="2"/>
+        <v>6098000</v>
+      </c>
+      <c r="D188" s="6">
+        <v>81264</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="9">
+        <v>44049</v>
+      </c>
+      <c r="B189" s="6">
+        <v>6182</v>
+      </c>
+      <c r="C189" s="6">
+        <f t="shared" si="2"/>
+        <v>6182000</v>
+      </c>
+      <c r="D189" s="6">
+        <v>82651</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="9">
+        <v>44050</v>
+      </c>
+      <c r="B190" s="6">
+        <v>6271</v>
+      </c>
+      <c r="C190" s="6">
+        <f t="shared" si="2"/>
+        <v>6271000</v>
+      </c>
+      <c r="D190" s="6">
+        <v>84761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>